<commit_message>
LPAD Linguagem de programção aplicado a dados
</commit_message>
<xml_diff>
--- a/LPAD_Linguagem_de_programcao_aplicado_a_dados/Vendas_01.xlsx
+++ b/LPAD_Linguagem_de_programcao_aplicado_a_dados/Vendas_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84284528572\OneDrive\Documentos\GitHub\Segundo_Semestre_Ciencia_de_Dados\LPAD_Linguagem_de_programcao_aplicado_a_dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa502bea7be57193/Documentos/GitHub/Segundo_Semestre_Ciencia_de_Dados/LPAD_Linguagem_de_programcao_aplicado_a_dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E3623D6B-BC77-453F-82A0-07293A8D80DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1B9F36A-66D5-4944-B55D-3D3384C9D5B8}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{E3623D6B-BC77-453F-82A0-07293A8D80DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6BA888B-E711-4298-9C6D-B658E9B376D2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -150,17 +150,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -178,6 +177,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2159,7 +2162,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F58" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A2:F58">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F58">
       <sortCondition ref="D1:D58"/>
     </sortState>
   </autoFilter>
@@ -2172,7 +2175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB86D40-21E3-4EBE-846A-CA430225F4F7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2199,7 +2202,7 @@
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7">
+      <c r="B1" s="6">
         <v>150</v>
       </c>
     </row>
@@ -2226,10 +2229,10 @@
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>2</v>
       </c>
     </row>
@@ -2237,10 +2240,10 @@
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>2</v>
       </c>
     </row>
@@ -2248,10 +2251,10 @@
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
@@ -2259,10 +2262,10 @@
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <v>4</v>
       </c>
     </row>
@@ -2270,10 +2273,10 @@
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>9</v>
       </c>
     </row>

</xml_diff>